<commit_message>
Removed unnecessary files from SaltedFiles/Default to reduce clutter and improve performance.
</commit_message>
<xml_diff>
--- a/config/Programs.xlsx
+++ b/config/Programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mike_\GitHub\Cybersec\Cybersec-practice\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1B261A-E232-406A-81D8-079A0B1A0872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357EABD0-B785-4DA3-901D-FB7205D8FC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1065" yWindow="4515" windowWidth="14730" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,6 +42,7 @@
     <author>tc={68BC9ABD-A73C-42DF-90C7-CA7FC2BFE757}</author>
     <author>tc={49D2EAE8-6B4E-47FB-9F94-6F66DACA1B90}</author>
     <author>tc={C1542AB1-4F61-452D-BB8A-01AB0387EBDA}</author>
+    <author>tc={E5648C2A-07E0-4434-8E8C-C600CAB8B365}</author>
   </authors>
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{97579503-219D-4842-B481-A01C26B7D412}">
@@ -76,12 +77,20 @@
     This column is where you input the registry or filepath to validate the program.  Registry paths need to use HKLM:\ or HKCU:\ for verification to work</t>
       </text>
     </comment>
+    <comment ref="M1" authorId="4" shapeId="0" xr:uid="{E5648C2A-07E0-4434-8E8C-C600CAB8B365}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Set to Yes if the appplication does not support -wait, but you still need to pause before continuing.  This helps to delay the Loading screen from disappearing prematurely.</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="98">
   <si>
     <t>Filename</t>
   </si>
@@ -372,13 +381,16 @@
   </si>
   <si>
     <t>HKLM:\SOFTWARE\WOW6432Node\Microsoft\Windows\CurrentVersion\Uninstall\{D5C6DB0C-BC43-4A77-9121-D1A07591F855}_is1</t>
+  </si>
+  <si>
+    <t>ForceWait</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,6 +405,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -757,15 +775,18 @@
   <threadedComment ref="H1" dT="2025-08-25T21:57:12.48" personId="{8CD43C30-B79F-4B57-A474-DA8EC33DFB12}" id="{C1542AB1-4F61-452D-BB8A-01AB0387EBDA}">
     <text>This column is where you input the registry or filepath to validate the program.  Registry paths need to use HKLM:\ or HKCU:\ for verification to work</text>
   </threadedComment>
+  <threadedComment ref="M1" dT="2025-11-04T20:38:21.89" personId="{8CD43C30-B79F-4B57-A474-DA8EC33DFB12}" id="{E5648C2A-07E0-4434-8E8C-C600CAB8B365}">
+    <text>Set to Yes if the appplication does not support -wait, but you still need to pause before continuing.  This helps to delay the Loading screen from disappearing prematurely.</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection sqref="A1:L2"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +798,7 @@
     <col min="8" max="8" width="126.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -814,8 +835,11 @@
       <c r="L1" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -841,7 +865,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -867,7 +891,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -893,7 +917,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -919,7 +943,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -945,7 +969,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -971,7 +995,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1003,7 +1027,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1029,7 +1053,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1067,7 +1091,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1093,7 +1117,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1125,7 +1149,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1163,7 +1187,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1189,7 +1213,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1215,7 +1239,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1241,7 +1265,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1279,7 +1303,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1305,7 +1329,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1330,8 +1354,11 @@
       <c r="H19" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -1357,7 +1384,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1391,7 +1418,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G22 G24:G1048576" xr:uid="{0FFCB68B-FA9F-484E-85D0-16EF647486F4}">
       <formula1>"RegistryKey,File,Folder"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C22 C24:C1048576" xr:uid="{2DCA6A76-F09F-4404-9AB9-7BEB5DB38117}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C22 C24:C1048576 O1:O1048576 M2:M1048576" xr:uid="{2DCA6A76-F09F-4404-9AB9-7BEB5DB38117}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F22 F24:F1048576" xr:uid="{104019E6-74A2-4236-9297-DF66F6F580D3}">

</xml_diff>

<commit_message>
Ready for Alpha release - updated setup and scorecard scripts
</commit_message>
<xml_diff>
--- a/config/Programs.xlsx
+++ b/config/Programs.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mike_\GitHub\Cybersec\Cybersec-practice\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001EEDEC-5EAE-489D-ACA9-B2CA17BD5E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03B22C0-3D52-4139-9DB9-773E8FE4684B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8040" yWindow="3510" windowWidth="21960" windowHeight="10650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8235" yWindow="4155" windowWidth="21960" windowHeight="10650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Software" sheetId="1" r:id="rId1"/>
-    <sheet name="Totals" sheetId="2" r:id="rId2"/>
+    <sheet name="Software Categories" sheetId="3" r:id="rId2"/>
+    <sheet name="Totals" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -91,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="112">
   <si>
     <t>Filename</t>
   </si>
@@ -397,6 +398,36 @@
   </si>
   <si>
     <t>Total Manual Malware Programs</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>General, IT</t>
+  </si>
+  <si>
+    <t>Adventure, Mapping, Training</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Mapping</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Adventure</t>
   </si>
 </sst>
 </file>
@@ -505,6 +536,16 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Mike Law" id="{8CD43C30-B79F-4B57-A474-DA8EC33DFB12}" userId="98b7d5602d91b815" providerId="Windows Live"/>
 </personList>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B968332B-406B-43C4-8C8C-AEF4CCF97C0A}" name="Table1" displayName="Table1" ref="A1:A1048576" totalsRowShown="0">
+  <autoFilter ref="A1:A1048576" xr:uid="{B968332B-406B-43C4-8C8C-AEF4CCF97C0A}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{9B028EA3-A4D0-4B6F-9074-390FD0FE939F}" name="Category"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -790,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +846,7 @@
     <col min="8" max="8" width="126.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -845,8 +886,11 @@
       <c r="M1" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -871,8 +915,11 @@
       <c r="H2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -897,8 +944,11 @@
       <c r="H3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -923,8 +973,11 @@
       <c r="H4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -949,8 +1002,11 @@
       <c r="H5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -975,8 +1031,11 @@
       <c r="H6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1002,7 +1061,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1034,7 +1093,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1060,7 +1119,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1098,7 +1157,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1124,7 +1183,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1156,7 +1215,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1194,7 +1253,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1220,7 +1279,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1246,7 +1305,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1272,7 +1331,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1310,7 +1369,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1336,7 +1395,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1365,7 +1424,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -1391,7 +1450,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1416,10 +1475,13 @@
       <c r="H21" t="s">
         <v>94</v>
       </c>
+      <c r="N21" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H19 J19 L19" xr:uid="{8A252F29-8030-444F-B770-32BE651BD0B2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H19 J19 N19 L19" xr:uid="{8A252F29-8030-444F-B770-32BE651BD0B2}">
       <formula1>"Registry Key, File,Registry Value"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G22 G24:G1048576" xr:uid="{0FFCB68B-FA9F-484E-85D0-16EF647486F4}">
@@ -1442,6 +1504,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{634DEE5C-1F55-4607-8A39-A2716773C7B5}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C64430-FE6C-4714-B10E-3705B50E4586}">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>

<commit_message>
added program install overrides and debugging improvements
</commit_message>
<xml_diff>
--- a/config/Programs.xlsx
+++ b/config/Programs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mike_\GitHub\Cybersec\Cybersec-practice\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03B22C0-3D52-4139-9DB9-773E8FE4684B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946FC276-943B-4994-B056-2ACA5A2165D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8235" yWindow="4155" windowWidth="21960" windowHeight="10650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5925" yWindow="5685" windowWidth="21960" windowHeight="10650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Software" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="112">
   <si>
     <t>Filename</t>
   </si>
@@ -833,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,7 +1270,7 @@
         <v>51</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G14" t="s">
         <v>22</v>
@@ -1367,6 +1367,9 @@
       </c>
       <c r="L17" t="s">
         <v>90</v>
+      </c>
+      <c r="M17" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>